<commit_message>
fix home equity assurance dists
</commit_message>
<xml_diff>
--- a/resources/NamingTable.xlsx
+++ b/resources/NamingTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mstern\Documents\GitHub\effective_property_tax\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4807894F-3467-40B3-BE4F-0973AD83B059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F9D190-9BFE-45A7-AB7D-1B8D31AC050C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13230" uniqueCount="5832">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13233" uniqueCount="5833">
   <si>
     <t>County</t>
   </si>
@@ -17533,6 +17533,9 @@
   </si>
   <si>
     <t>154SSA</t>
+  </si>
+  <si>
+    <t>Home Equity Assurance District</t>
   </si>
 </sst>
 </file>
@@ -18060,8 +18063,8 @@
   <dimension ref="A1:F2959"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <pane ySplit="1" topLeftCell="A336" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B349" sqref="B349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23951,6 +23954,9 @@
       <c r="D349">
         <v>110040000</v>
       </c>
+      <c r="E349" t="s">
+        <v>5832</v>
+      </c>
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
@@ -23965,6 +23971,9 @@
       <c r="D350">
         <v>110030000</v>
       </c>
+      <c r="E350" t="s">
+        <v>5832</v>
+      </c>
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
@@ -26137,6 +26146,9 @@
       </c>
       <c r="D478">
         <v>110020000</v>
+      </c>
+      <c r="E478" t="s">
+        <v>5832</v>
       </c>
     </row>
     <row r="479" spans="1:5" x14ac:dyDescent="0.3">
@@ -47986,7 +47998,7 @@
         <v>60</v>
       </c>
       <c r="F1798" t="str">
-        <f>C1798</f>
+        <f t="shared" ref="F1798:F1811" si="0">C1798</f>
         <v>VOLO SSA #9</v>
       </c>
     </row>
@@ -48004,7 +48016,7 @@
         <v>60</v>
       </c>
       <c r="F1799" t="str">
-        <f>C1799</f>
+        <f t="shared" si="0"/>
         <v>VOLO SSA #8</v>
       </c>
     </row>
@@ -48022,7 +48034,7 @@
         <v>60</v>
       </c>
       <c r="F1800" t="str">
-        <f>C1800</f>
+        <f t="shared" si="0"/>
         <v>VOLO SSA #6</v>
       </c>
     </row>
@@ -48040,7 +48052,7 @@
         <v>60</v>
       </c>
       <c r="F1801" t="str">
-        <f>C1801</f>
+        <f t="shared" si="0"/>
         <v>VOLO SSA #5</v>
       </c>
     </row>
@@ -48058,7 +48070,7 @@
         <v>60</v>
       </c>
       <c r="F1802" t="str">
-        <f>C1802</f>
+        <f t="shared" si="0"/>
         <v>VOLO SSA #4</v>
       </c>
     </row>
@@ -48076,7 +48088,7 @@
         <v>60</v>
       </c>
       <c r="F1803" t="str">
-        <f>C1803</f>
+        <f t="shared" si="0"/>
         <v>VOLO SSA #3</v>
       </c>
     </row>
@@ -48094,7 +48106,7 @@
         <v>60</v>
       </c>
       <c r="F1804" t="str">
-        <f>C1804</f>
+        <f t="shared" si="0"/>
         <v>VOLO SSA #2</v>
       </c>
     </row>
@@ -48112,7 +48124,7 @@
         <v>60</v>
       </c>
       <c r="F1805" t="str">
-        <f>C1805</f>
+        <f t="shared" si="0"/>
         <v>VOLO SSA #18</v>
       </c>
     </row>
@@ -48130,7 +48142,7 @@
         <v>60</v>
       </c>
       <c r="F1806" t="str">
-        <f>C1806</f>
+        <f t="shared" si="0"/>
         <v>VOLO SSA #17</v>
       </c>
     </row>
@@ -48148,7 +48160,7 @@
         <v>60</v>
       </c>
       <c r="F1807" t="str">
-        <f>C1807</f>
+        <f t="shared" si="0"/>
         <v>VOLO SSA #16</v>
       </c>
     </row>
@@ -48166,7 +48178,7 @@
         <v>60</v>
       </c>
       <c r="F1808" t="str">
-        <f>C1808</f>
+        <f t="shared" si="0"/>
         <v>VOLO SSA #15</v>
       </c>
     </row>
@@ -48184,7 +48196,7 @@
         <v>60</v>
       </c>
       <c r="F1809" t="str">
-        <f>C1809</f>
+        <f t="shared" si="0"/>
         <v>VOLO SSA #14</v>
       </c>
     </row>
@@ -48202,7 +48214,7 @@
         <v>60</v>
       </c>
       <c r="F1810" t="str">
-        <f>C1810</f>
+        <f t="shared" si="0"/>
         <v>VOLO SSA #11</v>
       </c>
     </row>
@@ -48220,7 +48232,7 @@
         <v>60</v>
       </c>
       <c r="F1811" t="str">
-        <f>C1811</f>
+        <f t="shared" si="0"/>
         <v>VOLO SSA #10</v>
       </c>
     </row>
@@ -48295,7 +48307,7 @@
         <v>60</v>
       </c>
       <c r="F1815" t="str">
-        <f>C1815</f>
+        <f t="shared" ref="F1815:F1820" si="1">C1815</f>
         <v>VERNON HILLS SSA #6</v>
       </c>
     </row>
@@ -48313,7 +48325,7 @@
         <v>60</v>
       </c>
       <c r="F1816" t="str">
-        <f>C1816</f>
+        <f t="shared" si="1"/>
         <v>VERNON HILLS SSA #5</v>
       </c>
     </row>
@@ -48331,7 +48343,7 @@
         <v>60</v>
       </c>
       <c r="F1817" t="str">
-        <f>C1817</f>
+        <f t="shared" si="1"/>
         <v>VERNON HILLS SSA #4</v>
       </c>
     </row>
@@ -48349,7 +48361,7 @@
         <v>60</v>
       </c>
       <c r="F1818" t="str">
-        <f>C1818</f>
+        <f t="shared" si="1"/>
         <v>VERNON HILLS SSA #3</v>
       </c>
     </row>
@@ -48367,7 +48379,7 @@
         <v>60</v>
       </c>
       <c r="F1819" t="str">
-        <f>C1819</f>
+        <f t="shared" si="1"/>
         <v>VERNON HILLS SSA #2</v>
       </c>
     </row>
@@ -48385,7 +48397,7 @@
         <v>60</v>
       </c>
       <c r="F1820" t="str">
-        <f>C1820</f>
+        <f t="shared" si="1"/>
         <v>VERNON HILLS SSA #1</v>
       </c>
     </row>
@@ -49394,7 +49406,7 @@
         <v>60</v>
       </c>
       <c r="F1879" t="str">
-        <f>C1879</f>
+        <f t="shared" ref="F1879:F1885" si="2">C1879</f>
         <v>ROUND LAKE SSA #4 - LAKEWOOD GROVE</v>
       </c>
     </row>
@@ -49412,7 +49424,7 @@
         <v>60</v>
       </c>
       <c r="F1880" t="str">
-        <f>C1880</f>
+        <f t="shared" si="2"/>
         <v>ROUND LAKE SSA #3 - LAKEWOOD GROVE</v>
       </c>
     </row>
@@ -49430,7 +49442,7 @@
         <v>60</v>
       </c>
       <c r="F1881" t="str">
-        <f>C1881</f>
+        <f t="shared" si="2"/>
         <v>ROUND LAKE SSA #2 - PW</v>
       </c>
     </row>
@@ -49448,7 +49460,7 @@
         <v>60</v>
       </c>
       <c r="F1882" t="str">
-        <f>C1882</f>
+        <f t="shared" si="2"/>
         <v>ROUND LAKE SSA #2 - LAKEWOOD GROVE</v>
       </c>
     </row>
@@ -49466,7 +49478,7 @@
         <v>60</v>
       </c>
       <c r="F1883" t="str">
-        <f>C1883</f>
+        <f t="shared" si="2"/>
         <v>ROUND LAKE SSA #1 - LAKEWOOD GROVE</v>
       </c>
     </row>
@@ -49484,7 +49496,7 @@
         <v>60</v>
       </c>
       <c r="F1884" t="str">
-        <f>C1884</f>
+        <f t="shared" si="2"/>
         <v>ROUND LAKE SSA #1 - BRIGHT MEADOWS</v>
       </c>
     </row>
@@ -49502,7 +49514,7 @@
         <v>60</v>
       </c>
       <c r="F1885" t="str">
-        <f>C1885</f>
+        <f t="shared" si="2"/>
         <v>ROUND LAKE SSA #1</v>
       </c>
     </row>
@@ -49765,7 +49777,7 @@
         <v>60</v>
       </c>
       <c r="F1899" t="str">
-        <f>C1899</f>
+        <f t="shared" ref="F1899:F1927" si="3">C1899</f>
         <v>RIVERWOODS SSA #9</v>
       </c>
     </row>
@@ -49783,7 +49795,7 @@
         <v>60</v>
       </c>
       <c r="F1900" t="str">
-        <f>C1900</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #8</v>
       </c>
     </row>
@@ -49801,7 +49813,7 @@
         <v>60</v>
       </c>
       <c r="F1901" t="str">
-        <f>C1901</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #7</v>
       </c>
     </row>
@@ -49819,7 +49831,7 @@
         <v>60</v>
       </c>
       <c r="F1902" t="str">
-        <f>C1902</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #6</v>
       </c>
     </row>
@@ -49837,7 +49849,7 @@
         <v>60</v>
       </c>
       <c r="F1903" t="str">
-        <f>C1903</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #5</v>
       </c>
     </row>
@@ -49855,7 +49867,7 @@
         <v>60</v>
       </c>
       <c r="F1904" t="str">
-        <f>C1904</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #4</v>
       </c>
     </row>
@@ -49873,7 +49885,7 @@
         <v>60</v>
       </c>
       <c r="F1905" t="str">
-        <f>C1905</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #32</v>
       </c>
     </row>
@@ -49891,7 +49903,7 @@
         <v>60</v>
       </c>
       <c r="F1906" t="str">
-        <f>C1906</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #31</v>
       </c>
     </row>
@@ -49909,7 +49921,7 @@
         <v>60</v>
       </c>
       <c r="F1907" t="str">
-        <f>C1907</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #30</v>
       </c>
     </row>
@@ -49927,7 +49939,7 @@
         <v>60</v>
       </c>
       <c r="F1908" t="str">
-        <f>C1908</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #3</v>
       </c>
     </row>
@@ -49945,7 +49957,7 @@
         <v>60</v>
       </c>
       <c r="F1909" t="str">
-        <f>C1909</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #29</v>
       </c>
     </row>
@@ -49963,7 +49975,7 @@
         <v>60</v>
       </c>
       <c r="F1910" t="str">
-        <f>C1910</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #28</v>
       </c>
     </row>
@@ -49981,7 +49993,7 @@
         <v>60</v>
       </c>
       <c r="F1911" t="str">
-        <f>C1911</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #27</v>
       </c>
     </row>
@@ -49999,7 +50011,7 @@
         <v>60</v>
       </c>
       <c r="F1912" t="str">
-        <f>C1912</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #26</v>
       </c>
     </row>
@@ -50017,7 +50029,7 @@
         <v>60</v>
       </c>
       <c r="F1913" t="str">
-        <f>C1913</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #25</v>
       </c>
     </row>
@@ -50035,7 +50047,7 @@
         <v>60</v>
       </c>
       <c r="F1914" t="str">
-        <f>C1914</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #24</v>
       </c>
     </row>
@@ -50053,7 +50065,7 @@
         <v>60</v>
       </c>
       <c r="F1915" t="str">
-        <f>C1915</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #23</v>
       </c>
     </row>
@@ -50071,7 +50083,7 @@
         <v>60</v>
       </c>
       <c r="F1916" t="str">
-        <f>C1916</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #22</v>
       </c>
     </row>
@@ -50089,7 +50101,7 @@
         <v>60</v>
       </c>
       <c r="F1917" t="str">
-        <f>C1917</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #21</v>
       </c>
     </row>
@@ -50107,7 +50119,7 @@
         <v>60</v>
       </c>
       <c r="F1918" t="str">
-        <f>C1918</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #20</v>
       </c>
     </row>
@@ -50125,7 +50137,7 @@
         <v>60</v>
       </c>
       <c r="F1919" t="str">
-        <f>C1919</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #19</v>
       </c>
     </row>
@@ -50143,7 +50155,7 @@
         <v>60</v>
       </c>
       <c r="F1920" t="str">
-        <f>C1920</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #18</v>
       </c>
     </row>
@@ -50161,7 +50173,7 @@
         <v>60</v>
       </c>
       <c r="F1921" t="str">
-        <f>C1921</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #17</v>
       </c>
     </row>
@@ -50179,7 +50191,7 @@
         <v>60</v>
       </c>
       <c r="F1922" t="str">
-        <f>C1922</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #16</v>
       </c>
     </row>
@@ -50197,7 +50209,7 @@
         <v>60</v>
       </c>
       <c r="F1923" t="str">
-        <f>C1923</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #15</v>
       </c>
     </row>
@@ -50215,7 +50227,7 @@
         <v>60</v>
       </c>
       <c r="F1924" t="str">
-        <f>C1924</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #14</v>
       </c>
     </row>
@@ -50233,7 +50245,7 @@
         <v>60</v>
       </c>
       <c r="F1925" t="str">
-        <f>C1925</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #12</v>
       </c>
     </row>
@@ -50251,7 +50263,7 @@
         <v>60</v>
       </c>
       <c r="F1926" t="str">
-        <f>C1926</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #11</v>
       </c>
     </row>
@@ -50269,7 +50281,7 @@
         <v>60</v>
       </c>
       <c r="F1927" t="str">
-        <f>C1927</f>
+        <f t="shared" si="3"/>
         <v>RIVERWOODS SSA #10</v>
       </c>
     </row>
@@ -50460,7 +50472,7 @@
         <v>60</v>
       </c>
       <c r="F1937" t="str">
-        <f>C1937</f>
+        <f t="shared" ref="F1937:F1945" si="4">C1937</f>
         <v>NORTH BARRINGTON SSA #7</v>
       </c>
     </row>
@@ -50478,7 +50490,7 @@
         <v>60</v>
       </c>
       <c r="F1938" t="str">
-        <f>C1938</f>
+        <f t="shared" si="4"/>
         <v>NORTH BARRINGTON SSA #6</v>
       </c>
     </row>
@@ -50496,7 +50508,7 @@
         <v>60</v>
       </c>
       <c r="F1939" t="str">
-        <f>C1939</f>
+        <f t="shared" si="4"/>
         <v>NORTH BARRINGTON SSA #5</v>
       </c>
     </row>
@@ -50514,7 +50526,7 @@
         <v>60</v>
       </c>
       <c r="F1940" t="str">
-        <f>C1940</f>
+        <f t="shared" si="4"/>
         <v>NORTH BARRINGTON SSA #18</v>
       </c>
     </row>
@@ -50532,7 +50544,7 @@
         <v>60</v>
       </c>
       <c r="F1941" t="str">
-        <f>C1941</f>
+        <f t="shared" si="4"/>
         <v>NORTH BARRINGTON SSA #18</v>
       </c>
     </row>
@@ -50550,7 +50562,7 @@
         <v>60</v>
       </c>
       <c r="F1942" t="str">
-        <f>C1942</f>
+        <f t="shared" si="4"/>
         <v>NORTH BARRINGTON SSA #17</v>
       </c>
     </row>
@@ -50568,7 +50580,7 @@
         <v>60</v>
       </c>
       <c r="F1943" t="str">
-        <f>C1943</f>
+        <f t="shared" si="4"/>
         <v>NORTH BARRINGTON SSA #15</v>
       </c>
     </row>
@@ -50586,7 +50598,7 @@
         <v>60</v>
       </c>
       <c r="F1944" t="str">
-        <f>C1944</f>
+        <f t="shared" si="4"/>
         <v>NORTH BARRINGTON SSA #14</v>
       </c>
     </row>
@@ -50604,7 +50616,7 @@
         <v>60</v>
       </c>
       <c r="F1945" t="str">
-        <f>C1945</f>
+        <f t="shared" si="4"/>
         <v>NORTH BARRINGTON SSA #13</v>
       </c>
     </row>
@@ -50793,7 +50805,7 @@
         <v>60</v>
       </c>
       <c r="F1955" t="str">
-        <f>C1955</f>
+        <f t="shared" ref="F1955:F1966" si="5">C1955</f>
         <v>METTAWA SSA #8Z</v>
       </c>
     </row>
@@ -50811,7 +50823,7 @@
         <v>60</v>
       </c>
       <c r="F1956" t="str">
-        <f>C1956</f>
+        <f t="shared" si="5"/>
         <v>METTAWA SSA #8Y</v>
       </c>
     </row>
@@ -50829,7 +50841,7 @@
         <v>60</v>
       </c>
       <c r="F1957" t="str">
-        <f>C1957</f>
+        <f t="shared" si="5"/>
         <v>METTAWA SSA #8X</v>
       </c>
     </row>
@@ -50847,7 +50859,7 @@
         <v>60</v>
       </c>
       <c r="F1958" t="str">
-        <f>C1958</f>
+        <f t="shared" si="5"/>
         <v>METTAWA SSA #8W</v>
       </c>
     </row>
@@ -50865,7 +50877,7 @@
         <v>60</v>
       </c>
       <c r="F1959" t="str">
-        <f>C1959</f>
+        <f t="shared" si="5"/>
         <v>METTAWA SSA #8V</v>
       </c>
     </row>
@@ -50883,7 +50895,7 @@
         <v>60</v>
       </c>
       <c r="F1960" t="str">
-        <f>C1960</f>
+        <f t="shared" si="5"/>
         <v>METTAWA SSA #8U</v>
       </c>
     </row>
@@ -50901,7 +50913,7 @@
         <v>60</v>
       </c>
       <c r="F1961" t="str">
-        <f>C1961</f>
+        <f t="shared" si="5"/>
         <v>METTAWA SSA #8T</v>
       </c>
     </row>
@@ -50919,7 +50931,7 @@
         <v>60</v>
       </c>
       <c r="F1962" t="str">
-        <f>C1962</f>
+        <f t="shared" si="5"/>
         <v>METTAWA SSA #8S</v>
       </c>
     </row>
@@ -50937,7 +50949,7 @@
         <v>60</v>
       </c>
       <c r="F1963" t="str">
-        <f>C1963</f>
+        <f t="shared" si="5"/>
         <v>METTAWA SSA #8R</v>
       </c>
     </row>
@@ -50955,7 +50967,7 @@
         <v>60</v>
       </c>
       <c r="F1964" t="str">
-        <f>C1964</f>
+        <f t="shared" si="5"/>
         <v>METTAWA SSA #8Q</v>
       </c>
     </row>
@@ -50973,7 +50985,7 @@
         <v>60</v>
       </c>
       <c r="F1965" t="str">
-        <f>C1965</f>
+        <f t="shared" si="5"/>
         <v>METTAWA SSA #8P</v>
       </c>
     </row>
@@ -50991,7 +51003,7 @@
         <v>60</v>
       </c>
       <c r="F1966" t="str">
-        <f>C1966</f>
+        <f t="shared" si="5"/>
         <v>METTAWA SSA #8O</v>
       </c>
     </row>
@@ -51516,7 +51528,7 @@
         <v>60</v>
       </c>
       <c r="F1996" t="str">
-        <f>C1996</f>
+        <f t="shared" ref="F1996:F2010" si="6">C1996</f>
         <v>METTAWA SSA #6Q</v>
       </c>
     </row>
@@ -51534,7 +51546,7 @@
         <v>60</v>
       </c>
       <c r="F1997" t="str">
-        <f>C1997</f>
+        <f t="shared" si="6"/>
         <v>METTAWA SSA #6P</v>
       </c>
     </row>
@@ -51552,7 +51564,7 @@
         <v>60</v>
       </c>
       <c r="F1998" t="str">
-        <f>C1998</f>
+        <f t="shared" si="6"/>
         <v>METTAWA SSA #6O</v>
       </c>
     </row>
@@ -51570,7 +51582,7 @@
         <v>60</v>
       </c>
       <c r="F1999" t="str">
-        <f>C1999</f>
+        <f t="shared" si="6"/>
         <v>METTAWA SSA #6N</v>
       </c>
     </row>
@@ -51588,7 +51600,7 @@
         <v>60</v>
       </c>
       <c r="F2000" t="str">
-        <f>C2000</f>
+        <f t="shared" si="6"/>
         <v>METTAWA SSA #6M</v>
       </c>
     </row>
@@ -51606,7 +51618,7 @@
         <v>60</v>
       </c>
       <c r="F2001" t="str">
-        <f>C2001</f>
+        <f t="shared" si="6"/>
         <v>METTAWA SSA #6L</v>
       </c>
     </row>
@@ -51624,7 +51636,7 @@
         <v>60</v>
       </c>
       <c r="F2002" t="str">
-        <f>C2002</f>
+        <f t="shared" si="6"/>
         <v>METTAWA SSA #6K</v>
       </c>
     </row>
@@ -51642,7 +51654,7 @@
         <v>60</v>
       </c>
       <c r="F2003" t="str">
-        <f>C2003</f>
+        <f t="shared" si="6"/>
         <v>METTAWA SSA #6J</v>
       </c>
     </row>
@@ -51660,7 +51672,7 @@
         <v>60</v>
       </c>
       <c r="F2004" t="str">
-        <f>C2004</f>
+        <f t="shared" si="6"/>
         <v>METTAWA SSA #6I</v>
       </c>
     </row>
@@ -51678,7 +51690,7 @@
         <v>60</v>
       </c>
       <c r="F2005" t="str">
-        <f>C2005</f>
+        <f t="shared" si="6"/>
         <v>METTAWA SSA #6H</v>
       </c>
     </row>
@@ -51696,7 +51708,7 @@
         <v>60</v>
       </c>
       <c r="F2006" t="str">
-        <f>C2006</f>
+        <f t="shared" si="6"/>
         <v>METTAWA SSA #6G</v>
       </c>
     </row>
@@ -51714,7 +51726,7 @@
         <v>60</v>
       </c>
       <c r="F2007" t="str">
-        <f>C2007</f>
+        <f t="shared" si="6"/>
         <v>METTAWA SSA #6F</v>
       </c>
     </row>
@@ -51732,7 +51744,7 @@
         <v>60</v>
       </c>
       <c r="F2008" t="str">
-        <f>C2008</f>
+        <f t="shared" si="6"/>
         <v>METTAWA SSA #6E</v>
       </c>
     </row>
@@ -51750,7 +51762,7 @@
         <v>60</v>
       </c>
       <c r="F2009" t="str">
-        <f>C2009</f>
+        <f t="shared" si="6"/>
         <v>METTAWA SSA #6D</v>
       </c>
     </row>
@@ -51768,7 +51780,7 @@
         <v>60</v>
       </c>
       <c r="F2010" t="str">
-        <f>C2010</f>
+        <f t="shared" si="6"/>
         <v>METTAWA SSA #6C</v>
       </c>
     </row>

</xml_diff>